<commit_message>
Cambios realizados para establecer estilos en resumen masivo temporales
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/plantillas/Resumen_masivo.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/plantillas/Resumen_masivo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20340"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AF635F-C5A7-4C0B-A6F3-E2AC06E1C6F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE4B612-95CB-4D04-A00F-390E984CD2D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,7 +79,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -87,23 +86,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -194,16 +178,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -216,11 +193,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -561,71 +539,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="28" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="25" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -634,5 +610,6 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="14" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>